<commit_message>
add user id to excel
</commit_message>
<xml_diff>
--- a/Student Metadata.xlsx
+++ b/Student Metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,26 +479,31 @@
           <t>Status Mahasiswa Saat ini</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>user_id</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MUHAMMAD AKMALUL IMAN LIARI</t>
+          <t>Syifa Khaista Khairunnisa</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Laki-Laki</t>
+          <t>Perempuan</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Universitas Pendidikan Indonesia</t>
+          <t>Universitas Indonesia</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Pendidikan Geografi</t>
+          <t>Teknik Kimia</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -507,11 +512,11 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>1900909</v>
+        <v>1706064012</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Ganjil 2019</t>
+          <t>Ganjil 2017</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -524,49 +529,9 @@
           <t>Belum Lulus</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Syifa Khaista Khairunnisa</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Perempuan</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Universitas Indonesia</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Teknik Kimia</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>1706064012</v>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Ganjil 2017</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Peserta didik baru</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Belum Lulus</t>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>U2020-0056</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add univ to filter
</commit_message>
<xml_diff>
--- a/Student Metadata.xlsx
+++ b/Student Metadata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,6 +535,58 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ADAM HAIKAL</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Laki-Laki</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Universitas Halu Oleo</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Ilmu Hukum</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>H1A117524</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ganjil 2017</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Peserta didik baru</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Belum Lulus</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>U2021-0003</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>